<commit_message>
UI modification for diployment
</commit_message>
<xml_diff>
--- a/Prompt.xlsx
+++ b/Prompt.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\AI_Projects\InternShipProjects\RAGify - RAG Concepts Quiz App\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\AI_Projects\InternShipProjects\RAGify---RAG-Concepts-Quiz-App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{507541BE-E5C4-4F40-A7ED-770A6FA8A84E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A3E3B2-CFE7-457C-B1DA-2CE37E693FC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
   </si>
   <si>
     <t xml:space="preserve">*"You are an AI quiz generator specializing in Retrieval-Augmented Generation (RAG). Create a quiz that tests a user,s understanding of RAG concepts, components, and workflows. 
-The quiz should include:
+The quiz should include :
     &gt;&gt;Multiple-choice questions = MCQ
     &gt;&gt;True/False questions=TF
     &gt;&gt;Short-answer questions=SAQ
@@ -83,6 +83,7 @@
             - SAQ: Check if the answer contains the core concept related to the question.
         3. Output Format:
             - Respond with either **Correct** or **Incorrect**.
+            -  Question No should start from 1 not 0
             {{"Question No": "  ",
             "Question " : "     ",
             "User Answer": "   ",
@@ -133,7 +134,9 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,7 +420,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,7 +437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -442,7 +445,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>

</xml_diff>